<commit_message>
Adding logic for interventions of electrification
</commit_message>
<xml_diff>
--- a/data/Interventions_One_Federal_source.xlsx
+++ b/data/Interventions_One_Federal_source.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulr\Documents\R\NCZ_Interventions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6029C1-289B-42E6-99FF-311AF94DA2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538B4317-399F-47CA-9FE1-D39B34556D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{73048387-4E92-4906-81CA-9C6189A709FA}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="59">
   <si>
     <t>Building Level Interventions</t>
   </si>
@@ -204,15 +204,9 @@
     <t>Optional add to elevator package</t>
   </si>
   <si>
-    <t xml:space="preserve">Electric Chillers </t>
-  </si>
-  <si>
     <t>Electric driveline for chillers</t>
   </si>
   <si>
-    <t>At bathroom upgrades</t>
-  </si>
-  <si>
     <t>caulking and general air stopping</t>
   </si>
   <si>
@@ -231,15 +225,6 @@
     <t>Insulation at TI's</t>
   </si>
   <si>
-    <t>AHU coils, and ASHP hot water for induction systems</t>
-  </si>
-  <si>
-    <t>AHU coils, and elect HW boiler  for induction systems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electric boiler </t>
-  </si>
-  <si>
     <t>Heating &amp; Cooling &amp; Base</t>
   </si>
   <si>
@@ -271,6 +256,9 @@
   </si>
   <si>
     <t>One Federal</t>
+  </si>
+  <si>
+    <t>Electrificaiton</t>
   </si>
 </sst>
 </file>
@@ -993,7 +981,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1003,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF149E70-DC8C-4A8D-84BB-B0051DA57024}">
   <dimension ref="A2:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1140,13 +1128,13 @@
     </row>
     <row r="17" spans="1:16" ht="63" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>2</v>
@@ -1190,16 +1178,16 @@
     </row>
     <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C18" s="18">
         <v>1</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>30</v>
@@ -1235,12 +1223,12 @@
         <v>16</v>
       </c>
       <c r="P18" s="23" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>34</v>
@@ -1285,12 +1273,12 @@
         <v>16</v>
       </c>
       <c r="P19" s="23" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>32</v>
@@ -1335,12 +1323,12 @@
         <v>16</v>
       </c>
       <c r="P20" s="23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>33</v>
@@ -1386,12 +1374,12 @@
         <v>16</v>
       </c>
       <c r="P21" s="23" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>32</v>
@@ -1403,7 +1391,7 @@
         <v>25</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>23</v>
@@ -1437,12 +1425,12 @@
         <v>16</v>
       </c>
       <c r="P22" s="23" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>32</v>
@@ -1454,7 +1442,7 @@
         <v>24</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F23" s="19" t="s">
         <v>23</v>
@@ -1467,13 +1455,13 @@
         <v>15</v>
       </c>
       <c r="I23" s="17">
-        <v>-0.25</v>
+        <v>3.5</v>
       </c>
       <c r="J23" s="17">
         <v>0</v>
       </c>
       <c r="K23" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L23" s="19">
         <v>30</v>
@@ -1488,12 +1476,12 @@
         <v>16</v>
       </c>
       <c r="P23" s="23" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>33</v>
@@ -1505,7 +1493,7 @@
         <v>28</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="F24" s="19" t="s">
         <v>18</v>
@@ -1544,7 +1532,7 @@
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>34</v>
@@ -1556,7 +1544,7 @@
         <v>29</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F25" s="19" t="s">
         <v>17</v>
@@ -1595,7 +1583,7 @@
     </row>
     <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>34</v>
@@ -1604,10 +1592,10 @@
         <v>8</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>18</v>
@@ -1646,7 +1634,7 @@
     </row>
     <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>34</v>
@@ -1655,10 +1643,10 @@
         <v>9</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F27" s="19" t="s">
         <v>18</v>
@@ -1697,7 +1685,7 @@
     </row>
     <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>31</v>
@@ -1709,7 +1697,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="F28" s="19" t="s">
         <v>23</v>
@@ -1722,7 +1710,7 @@
         <v>15</v>
       </c>
       <c r="I28" s="17">
-        <v>-0.7</v>
+        <v>2</v>
       </c>
       <c r="J28" s="17">
         <v>0</v>
@@ -1748,7 +1736,7 @@
     </row>
     <row r="29" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>31</v>
@@ -1760,7 +1748,7 @@
         <v>37</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F29" s="19" t="s">
         <v>23</v>
@@ -1773,7 +1761,7 @@
         <v>15</v>
       </c>
       <c r="I29" s="17">
-        <v>-0.9</v>
+        <v>1.05</v>
       </c>
       <c r="J29" s="17">
         <v>0</v>
@@ -1799,7 +1787,7 @@
     </row>
     <row r="30" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>31</v>
@@ -1808,10 +1796,10 @@
         <v>10</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F30" s="19" t="s">
         <v>23</v>
@@ -1823,7 +1811,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="17">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="J30" s="17">
         <v>0</v>
@@ -2176,7 +2164,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logic on populating savings columns
</commit_message>
<xml_diff>
--- a/data/Interventions_One_Federal_source.xlsx
+++ b/data/Interventions_One_Federal_source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulr\Documents\R\NCZ_Interventions\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7030BBB7-173A-4394-9DFD-CC14D5F30F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{7030BBB7-173A-4394-9DFD-CC14D5F30F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC5370C6-7089-4064-A0E7-8B7593DCACA4}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{73048387-4E92-4906-81CA-9C6189A709FA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{73048387-4E92-4906-81CA-9C6189A709FA}"/>
   </bookViews>
   <sheets>
     <sheet name="One Fed" sheetId="1" r:id="rId1"/>
@@ -989,34 +989,34 @@
   <dimension ref="A2:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.265625" customWidth="1"/>
-    <col min="3" max="3" width="5.19921875" customWidth="1"/>
-    <col min="4" max="4" width="35.19921875" customWidth="1"/>
-    <col min="5" max="5" width="36.53125" customWidth="1"/>
-    <col min="6" max="6" width="29.46484375" customWidth="1"/>
-    <col min="7" max="7" width="25.53125" customWidth="1"/>
-    <col min="8" max="8" width="15.19921875" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" customWidth="1"/>
+    <col min="5" max="5" width="36.54296875" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" customWidth="1"/>
+    <col min="7" max="7" width="25.54296875" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="21.265625" customWidth="1"/>
-    <col min="11" max="11" width="18.73046875" customWidth="1"/>
-    <col min="12" max="12" width="16.46484375" customWidth="1"/>
-    <col min="13" max="13" width="16.53125" customWidth="1"/>
-    <col min="14" max="14" width="20.19921875" customWidth="1"/>
-    <col min="15" max="15" width="14.73046875" customWidth="1"/>
-    <col min="16" max="16" width="26.19921875" customWidth="1"/>
+    <col min="10" max="10" width="21.26953125" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" customWidth="1"/>
+    <col min="14" max="14" width="20.1796875" customWidth="1"/>
+    <col min="15" max="15" width="14.7265625" customWidth="1"/>
+    <col min="16" max="16" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:16" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="3:16" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="3:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="25" t="s">
         <v>1</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="H4" s="26"/>
       <c r="I4" s="27"/>
     </row>
-    <row r="5" spans="3:16" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C5"/>
       <c r="D5" s="28"/>
       <c r="E5" s="29"/>
@@ -1042,7 +1042,7 @@
       <c r="O5"/>
       <c r="P5"/>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C6" s="3"/>
       <c r="D6" s="28"/>
       <c r="E6" s="29"/>
@@ -1051,7 +1051,7 @@
       <c r="H6" s="29"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D7" s="28"/>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
@@ -1059,7 +1059,7 @@
       <c r="H7" s="29"/>
       <c r="I7" s="30"/>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
@@ -1067,7 +1067,7 @@
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D9" s="28"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
@@ -1075,7 +1075,7 @@
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
     </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D10" s="28"/>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
@@ -1083,7 +1083,7 @@
       <c r="H10" s="29"/>
       <c r="I10" s="30"/>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D11" s="28"/>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
@@ -1091,7 +1091,7 @@
       <c r="H11" s="29"/>
       <c r="I11" s="30"/>
     </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D12" s="28"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
@@ -1099,7 +1099,7 @@
       <c r="H12" s="29"/>
       <c r="I12" s="30"/>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D13" s="28"/>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
@@ -1107,7 +1107,7 @@
       <c r="H13" s="29"/>
       <c r="I13" s="30"/>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D14" s="28"/>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
@@ -1115,7 +1115,7 @@
       <c r="H14" s="29"/>
       <c r="I14" s="30"/>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D15" s="31"/>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
@@ -1123,7 +1123,7 @@
       <c r="H15" s="32"/>
       <c r="I15" s="33"/>
     </row>
-    <row r="17" spans="1:16" ht="63" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:16" ht="62" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>15</v>
       </c>
       <c r="I22" s="17">
-        <v>-0.25</v>
+        <v>-0.8</v>
       </c>
       <c r="J22" s="17">
         <v>0</v>
@@ -1425,7 +1425,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>15</v>
       </c>
       <c r="I23" s="17">
-        <v>3.5</v>
+        <v>-0.65</v>
       </c>
       <c r="J23" s="17">
         <v>0</v>
@@ -1476,7 +1476,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>56</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>15</v>
       </c>
       <c r="I28" s="17">
-        <v>2</v>
+        <v>-1.5</v>
       </c>
       <c r="J28" s="17">
         <v>0</v>
@@ -1731,7 +1731,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>15</v>
       </c>
       <c r="I29" s="17">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="J29" s="17">
         <v>0</v>
@@ -1782,7 +1782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>19</v>
       </c>
       <c r="I30" s="17">
-        <v>1.05</v>
+        <v>-0.9</v>
       </c>
       <c r="J30" s="17">
         <v>0</v>
@@ -1832,7 +1832,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
@@ -1847,7 +1847,7 @@
       <c r="O31" s="22"/>
       <c r="P31" s="23"/>
     </row>
-    <row r="32" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
@@ -1862,7 +1862,7 @@
       <c r="O32" s="22"/>
       <c r="P32" s="23"/>
     </row>
-    <row r="33" spans="4:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
@@ -1877,7 +1877,7 @@
       <c r="O33" s="22"/>
       <c r="P33" s="23"/>
     </row>
-    <row r="34" spans="4:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="4:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
@@ -1892,7 +1892,7 @@
       <c r="O34" s="22"/>
       <c r="P34" s="23"/>
     </row>
-    <row r="35" spans="4:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="4:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
@@ -1907,7 +1907,7 @@
       <c r="O35" s="22"/>
       <c r="P35" s="23"/>
     </row>
-    <row r="36" spans="4:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="4:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
@@ -1922,7 +1922,7 @@
       <c r="O36" s="22"/>
       <c r="P36" s="23"/>
     </row>
-    <row r="37" spans="4:16" s="18" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="4:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
@@ -1937,7 +1937,7 @@
       <c r="O37" s="22"/>
       <c r="P37" s="23"/>
     </row>
-    <row r="38" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="38" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -1952,7 +1952,7 @@
       <c r="O38" s="12"/>
       <c r="P38" s="13"/>
     </row>
-    <row r="39" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="39" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
@@ -1967,7 +1967,7 @@
       <c r="O39" s="12"/>
       <c r="P39" s="13"/>
     </row>
-    <row r="40" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="40" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
@@ -1982,7 +1982,7 @@
       <c r="O40" s="12"/>
       <c r="P40" s="13"/>
     </row>
-    <row r="41" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="41" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
@@ -1997,7 +1997,7 @@
       <c r="O41" s="12"/>
       <c r="P41" s="13"/>
     </row>
-    <row r="42" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="42" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
@@ -2012,7 +2012,7 @@
       <c r="O42" s="12"/>
       <c r="P42" s="13"/>
     </row>
-    <row r="43" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="43" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -2027,7 +2027,7 @@
       <c r="O43" s="12"/>
       <c r="P43" s="13"/>
     </row>
-    <row r="44" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -2042,7 +2042,7 @@
       <c r="O44" s="12"/>
       <c r="P44" s="13"/>
     </row>
-    <row r="45" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D45" s="8"/>
       <c r="E45" s="8" t="s">
         <v>20</v>
@@ -2059,7 +2059,7 @@
       <c r="O45" s="12"/>
       <c r="P45" s="13"/>
     </row>
-    <row r="46" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="46" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D46" s="8"/>
       <c r="E46" s="8" t="s">
         <v>20</v>
@@ -2078,7 +2078,7 @@
       <c r="O46" s="12"/>
       <c r="P46" s="13"/>
     </row>
-    <row r="47" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="47" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
@@ -2137,29 +2137,29 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Working with electrificaiton file
</commit_message>
<xml_diff>
--- a/data/Interventions_One_Federal_source.xlsx
+++ b/data/Interventions_One_Federal_source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="8_{7E2A0C6A-54A5-426B-8D0F-83B42C89CDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{740ADD58-150A-44D6-A033-E39E3A5AD394}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="8_{7E2A0C6A-54A5-426B-8D0F-83B42C89CDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E074C01C-FF28-410A-9EC8-EC4CD79567CB}"/>
   <bookViews>
-    <workbookView xWindow="30075" yWindow="1500" windowWidth="21600" windowHeight="11325" xr2:uid="{73048387-4E92-4906-81CA-9C6189A709FA}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="16920" windowHeight="10540" xr2:uid="{73048387-4E92-4906-81CA-9C6189A709FA}"/>
   </bookViews>
   <sheets>
     <sheet name="One Fed" sheetId="1" r:id="rId1"/>
@@ -665,14 +665,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -710,7 +706,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -816,7 +812,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -958,7 +954,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -968,35 +964,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF149E70-DC8C-4A8D-84BB-B0051DA57024}">
   <dimension ref="A2:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="F12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" customWidth="1"/>
+    <col min="5" max="5" width="36.54296875" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" customWidth="1"/>
+    <col min="7" max="7" width="25.54296875" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="26.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.26953125" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" customWidth="1"/>
+    <col min="14" max="14" width="20.1796875" customWidth="1"/>
+    <col min="15" max="15" width="14.7265625" customWidth="1"/>
+    <col min="16" max="16" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:16" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="3:16" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.6">
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="25" t="s">
         <v>1</v>
       </c>
@@ -1006,7 +1002,7 @@
       <c r="H4" s="26"/>
       <c r="I4" s="27"/>
     </row>
-    <row r="5" spans="3:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C5"/>
       <c r="D5" s="28"/>
       <c r="E5" s="29"/>
@@ -1022,7 +1018,7 @@
       <c r="O5"/>
       <c r="P5"/>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C6" s="3"/>
       <c r="D6" s="28"/>
       <c r="E6" s="29"/>
@@ -1031,7 +1027,7 @@
       <c r="H6" s="29"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D7" s="28"/>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
@@ -1039,7 +1035,7 @@
       <c r="H7" s="29"/>
       <c r="I7" s="30"/>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
@@ -1047,7 +1043,7 @@
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D9" s="28"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
@@ -1055,7 +1051,7 @@
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
     </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D10" s="28"/>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
@@ -1063,7 +1059,7 @@
       <c r="H10" s="29"/>
       <c r="I10" s="30"/>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D11" s="28"/>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
@@ -1071,7 +1067,7 @@
       <c r="H11" s="29"/>
       <c r="I11" s="30"/>
     </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D12" s="28"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
@@ -1079,7 +1075,7 @@
       <c r="H12" s="29"/>
       <c r="I12" s="30"/>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D13" s="28"/>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
@@ -1087,7 +1083,7 @@
       <c r="H13" s="29"/>
       <c r="I13" s="30"/>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D14" s="28"/>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
@@ -1095,7 +1091,7 @@
       <c r="H14" s="29"/>
       <c r="I14" s="30"/>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.35">
       <c r="D15" s="31"/>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
@@ -1103,7 +1099,7 @@
       <c r="H15" s="32"/>
       <c r="I15" s="33"/>
     </row>
-    <row r="17" spans="1:16" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="62" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1153,7 +1149,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1193,7 +1189,7 @@
       <c r="O18" s="22"/>
       <c r="P18" s="23"/>
     </row>
-    <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1233,7 +1229,7 @@
       <c r="O19" s="22"/>
       <c r="P19" s="23"/>
     </row>
-    <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1273,7 +1269,7 @@
       <c r="O20" s="22"/>
       <c r="P20" s="23"/>
     </row>
-    <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1299,10 +1295,10 @@
         <v>45</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J21">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="K21" t="s">
         <v>46</v>
@@ -1313,7 +1309,7 @@
       <c r="O21" s="22"/>
       <c r="P21" s="23"/>
     </row>
-    <row r="22" spans="1:16" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="18" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1353,7 +1349,7 @@
       <c r="O22" s="22"/>
       <c r="P22" s="23"/>
     </row>
-    <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1393,7 +1389,7 @@
       <c r="O23" s="22"/>
       <c r="P23" s="23"/>
     </row>
-    <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1433,7 +1429,7 @@
       <c r="O24" s="22"/>
       <c r="P24" s="23"/>
     </row>
-    <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1473,7 +1469,7 @@
       <c r="O25" s="22"/>
       <c r="P25" s="23"/>
     </row>
-    <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1513,7 +1509,7 @@
       <c r="O26" s="22"/>
       <c r="P26" s="23"/>
     </row>
-    <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1553,7 +1549,7 @@
       <c r="O27" s="22"/>
       <c r="P27" s="23"/>
     </row>
-    <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
@@ -1569,7 +1565,7 @@
       <c r="O28" s="22"/>
       <c r="P28" s="23"/>
     </row>
-    <row r="29" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
@@ -1584,7 +1580,7 @@
       <c r="O29" s="22"/>
       <c r="P29" s="23"/>
     </row>
-    <row r="30" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
@@ -1599,7 +1595,7 @@
       <c r="O30" s="22"/>
       <c r="P30" s="23"/>
     </row>
-    <row r="31" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
@@ -1614,7 +1610,7 @@
       <c r="O31" s="22"/>
       <c r="P31" s="23"/>
     </row>
-    <row r="32" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
@@ -1629,7 +1625,7 @@
       <c r="O32" s="22"/>
       <c r="P32" s="23"/>
     </row>
-    <row r="33" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
@@ -1644,7 +1640,7 @@
       <c r="O33" s="22"/>
       <c r="P33" s="23"/>
     </row>
-    <row r="34" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
@@ -1659,7 +1655,7 @@
       <c r="O34" s="22"/>
       <c r="P34" s="23"/>
     </row>
-    <row r="35" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
@@ -1674,7 +1670,7 @@
       <c r="O35" s="22"/>
       <c r="P35" s="23"/>
     </row>
-    <row r="36" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
@@ -1689,7 +1685,7 @@
       <c r="O36" s="22"/>
       <c r="P36" s="23"/>
     </row>
-    <row r="37" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -1707,7 +1703,7 @@
       <c r="O37" s="12"/>
       <c r="P37" s="13"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -1722,7 +1718,7 @@
       <c r="O38" s="12"/>
       <c r="P38" s="13"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
@@ -1737,7 +1733,7 @@
       <c r="O39" s="12"/>
       <c r="P39" s="13"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D40" s="8"/>
       <c r="E40" s="8" t="s">
         <v>15</v>
@@ -1754,7 +1750,7 @@
       <c r="O40" s="12"/>
       <c r="P40" s="13"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D41" s="8"/>
       <c r="E41" s="8" t="s">
         <v>15</v>
@@ -1773,7 +1769,7 @@
       <c r="O41" s="12"/>
       <c r="P41" s="13"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
@@ -1788,7 +1784,7 @@
       <c r="O42" s="12"/>
       <c r="P42" s="16"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -1803,7 +1799,7 @@
       <c r="O43" s="12"/>
       <c r="P43" s="13"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -1818,7 +1814,7 @@
       <c r="O44" s="12"/>
       <c r="P44" s="13"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D45" s="8"/>
       <c r="E45" s="8" t="s">
         <v>15</v>
@@ -1835,7 +1831,7 @@
       <c r="O45" s="12"/>
       <c r="P45" s="13"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D46" s="8"/>
       <c r="E46" s="8" t="s">
         <v>15</v>
@@ -1854,7 +1850,7 @@
       <c r="O46" s="12"/>
       <c r="P46" s="13"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
@@ -1908,29 +1904,29 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
working on finishing this.
</commit_message>
<xml_diff>
--- a/data/Interventions_One_Federal_source.xlsx
+++ b/data/Interventions_One_Federal_source.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="563" documentId="8_{7E2A0C6A-54A5-426B-8D0F-83B42C89CDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74AD2F97-388F-42E6-8E5D-509CE7619DDB}"/>
+  <xr:revisionPtr revIDLastSave="576" documentId="8_{7E2A0C6A-54A5-426B-8D0F-83B42C89CDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9A3D215-31E8-4346-80EC-82A4DEB9572F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{73048387-4E92-4906-81CA-9C6189A709FA}"/>
   </bookViews>
   <sheets>
     <sheet name="One Fed" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="222 Second" sheetId="3" r:id="rId3"/>
-    <sheet name="160 Spear" sheetId="4" r:id="rId4"/>
+    <sheet name="222 N Lassalle" sheetId="6" r:id="rId3"/>
+    <sheet name="222 Second" sheetId="3" r:id="rId4"/>
+    <sheet name="160 Spear" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'One Fed'!$B$17:$P$27</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="74">
   <si>
     <t>Building Level Interventions</t>
   </si>
@@ -299,7 +300,13 @@
     <t>Chiller EOL Replacement</t>
   </si>
   <si>
-    <t>222 Second Street</t>
+    <t>222 N LaSalle</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Converge Network People counters </t>
   </si>
 </sst>
 </file>
@@ -741,6 +748,103 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1468976</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>175425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6A735AB-347D-4760-8C73-18216D22ACC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8076406" y="154781"/>
+          <a:ext cx="1457070" cy="573094"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1468976</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>29375</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B043CE7-319C-41CC-999A-2D94A273CA03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8076406" y="154781"/>
+          <a:ext cx="1457070" cy="573094"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1038,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF149E70-DC8C-4A8D-84BB-B0051DA57024}">
-  <dimension ref="A2:P43"/>
+  <dimension ref="A2:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1226,7 +1330,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B18" s="18" t="s">
@@ -1244,21 +1348,33 @@
       <c r="F18" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18">
-        <v>0.04</v>
-      </c>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="21"/>
+      <c r="G18" s="20">
+        <v>48000</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="25">
+        <v>138708</v>
+      </c>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="19">
+        <v>10</v>
+      </c>
+      <c r="M18" s="19">
+        <v>2025</v>
+      </c>
+      <c r="N18" s="21">
+        <v>0</v>
+      </c>
       <c r="O18" s="22"/>
-      <c r="P18" s="23"/>
+      <c r="P18" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -1268,27 +1384,40 @@
         <v>2</v>
       </c>
       <c r="D19" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="19"/>
       <c r="F19" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19">
+      <c r="G19" s="20">
+        <f>48660+2000000+35000</f>
+        <v>2083660</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="25">
         <v>0</v>
       </c>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19" s="19"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="19">
+        <v>15</v>
+      </c>
+      <c r="M19" s="19">
+        <v>2025</v>
+      </c>
       <c r="N19" s="21"/>
       <c r="O19" s="22"/>
-      <c r="P19" s="23"/>
+      <c r="P19" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B20" s="18" t="s">
@@ -1306,21 +1435,34 @@
       <c r="F20" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20">
-        <v>0.03</v>
-      </c>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="21"/>
+      <c r="G20" s="20">
+        <f>50000*4+12*25000</f>
+        <v>500000</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="25">
+        <v>2059819</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="19">
+        <v>15</v>
+      </c>
+      <c r="M20" s="19">
+        <v>2026</v>
+      </c>
+      <c r="N20" s="21">
+        <v>-15000</v>
+      </c>
       <c r="O20" s="22"/>
-      <c r="P20" s="23"/>
+      <c r="P20" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="18" t="s">
@@ -1338,21 +1480,31 @@
       <c r="F21" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21">
-        <v>0.02</v>
-      </c>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21" s="19"/>
+      <c r="G21" s="20">
+        <v>275000</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="25">
+        <v>230692</v>
+      </c>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="19">
+        <v>20</v>
+      </c>
+      <c r="M21" s="19">
+        <v>2025</v>
+      </c>
       <c r="N21" s="21"/>
       <c r="O21" s="22"/>
-      <c r="P21" s="23"/>
+      <c r="P21" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="18" t="s">
@@ -1370,21 +1522,32 @@
       <c r="F22" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22" s="19"/>
+      <c r="G22" s="20">
+        <f>1200000/1000*2400</f>
+        <v>2880000</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="25">
+        <v>572081</v>
+      </c>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="19">
+        <v>20</v>
+      </c>
+      <c r="M22" s="19">
+        <v>2028</v>
+      </c>
       <c r="N22" s="21"/>
       <c r="O22" s="22"/>
-      <c r="P22" s="23"/>
+      <c r="P22" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="18" t="s">
@@ -1402,21 +1565,31 @@
       <c r="F23" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23">
-        <v>0.02</v>
-      </c>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23" s="19"/>
+      <c r="G23" s="20">
+        <v>1300000</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="25">
+        <v>108695</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="19">
+        <v>15</v>
+      </c>
+      <c r="M23" s="19">
+        <v>2025</v>
+      </c>
       <c r="N23" s="21"/>
       <c r="O23" s="22"/>
-      <c r="P23" s="23"/>
+      <c r="P23" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B24" s="18" t="s">
@@ -1434,21 +1607,31 @@
       <c r="F24" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24">
-        <v>1E-3</v>
-      </c>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24" s="19"/>
+      <c r="G24" s="20">
+        <v>120000</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="25">
+        <v>19881</v>
+      </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="19">
+        <v>20</v>
+      </c>
+      <c r="M24" s="19">
+        <v>2025</v>
+      </c>
       <c r="N24" s="21"/>
       <c r="O24" s="22"/>
-      <c r="P24" s="23"/>
+      <c r="P24" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B25" s="18" t="s">
@@ -1466,21 +1649,32 @@
       <c r="F25" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25">
-        <v>1E-4</v>
-      </c>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25" s="19"/>
+      <c r="G25" s="20">
+        <f>39790*200</f>
+        <v>7958000</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="25">
+        <v>215217</v>
+      </c>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="19">
+        <v>35</v>
+      </c>
+      <c r="M25" s="19">
+        <v>2029</v>
+      </c>
       <c r="N25" s="21"/>
       <c r="O25" s="22"/>
-      <c r="P25" s="23"/>
+      <c r="P25" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="18" t="s">
@@ -1498,21 +1692,31 @@
       <c r="F26" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26">
-        <v>0.01</v>
-      </c>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26" s="19"/>
+      <c r="G26" s="20">
+        <v>400000</v>
+      </c>
+      <c r="H26" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="25">
+        <v>169502</v>
+      </c>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="19">
+        <v>25</v>
+      </c>
+      <c r="M26" s="19">
+        <v>2030</v>
+      </c>
       <c r="N26" s="21"/>
       <c r="O26" s="22"/>
-      <c r="P26" s="23"/>
+      <c r="P26" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B27" s="18" t="s">
@@ -1530,21 +1734,32 @@
       <c r="F27" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27">
-        <v>0.3</v>
-      </c>
-      <c r="J27"/>
-      <c r="K27"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
+      <c r="G27" s="20">
+        <f>3500*2*28</f>
+        <v>196000</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="25">
+        <v>16093</v>
+      </c>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="19">
+        <v>15</v>
+      </c>
+      <c r="M27" s="19">
+        <v>2025</v>
+      </c>
       <c r="N27" s="21"/>
       <c r="O27" s="22"/>
-      <c r="P27" s="23"/>
+      <c r="P27" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B28" s="18" t="s">
@@ -1562,21 +1777,32 @@
       <c r="F28" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="20"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="17">
-        <v>0.1</v>
+      <c r="G28" s="20">
+        <f>6*350000</f>
+        <v>2100000</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="25">
+        <v>32529</v>
       </c>
       <c r="J28" s="17"/>
       <c r="K28" s="17"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
+      <c r="L28" s="19">
+        <v>35</v>
+      </c>
+      <c r="M28" s="19">
+        <v>2025</v>
+      </c>
       <c r="N28" s="21"/>
       <c r="O28" s="22"/>
-      <c r="P28" s="23"/>
+      <c r="P28" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="29" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B29" s="18" t="s">
@@ -1592,23 +1818,33 @@
         <v>68</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="17">
-        <v>0.02</v>
+        <v>54</v>
+      </c>
+      <c r="G29" s="20">
+        <v>54100000</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="25">
+        <v>525655</v>
       </c>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
+      <c r="L29" s="19">
+        <v>40</v>
+      </c>
+      <c r="M29" s="19">
+        <v>2035</v>
+      </c>
       <c r="N29" s="21"/>
       <c r="O29" s="22"/>
-      <c r="P29" s="23"/>
+      <c r="P29" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="30" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B30" s="18" t="s">
@@ -1626,18 +1862,832 @@
       <c r="F30" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="17">
-        <v>0.15</v>
+      <c r="G30" s="20">
+        <f>1300*1500</f>
+        <v>1950000</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="25">
+        <v>383791</v>
       </c>
       <c r="J30" s="17"/>
       <c r="K30" s="17"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
+      <c r="L30" s="19">
+        <v>35</v>
+      </c>
+      <c r="M30" s="19">
+        <v>2030</v>
+      </c>
       <c r="N30" s="21"/>
       <c r="O30" s="22"/>
-      <c r="P30" s="23"/>
+      <c r="P30" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:P30">
+    <sortCondition ref="C18:C30"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="D4:I15"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26 H26 F28 O18:O30" xr:uid="{25478E18-0184-44CC-B842-F228497F826A}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2E54ED-FA3E-404F-B8C1-A4273C92F2A2}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BD6620-112F-45C6-AFAD-CCA1CA96DCC3}">
+  <dimension ref="A2:P43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="29.81640625" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" customWidth="1"/>
+    <col min="5" max="5" width="36.54296875" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" customWidth="1"/>
+    <col min="7" max="7" width="25.54296875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="21.26953125" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" customWidth="1"/>
+    <col min="14" max="14" width="20.1796875" customWidth="1"/>
+    <col min="15" max="15" width="14.7265625" customWidth="1"/>
+    <col min="16" max="16" width="26.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:16" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+    </row>
+    <row r="5" spans="3:16" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C5"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="C6" s="3"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="31"/>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="31"/>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D9" s="29"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="31"/>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D10" s="29"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D11" s="29"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31"/>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.35">
+      <c r="D15" s="32"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="34"/>
+    </row>
+    <row r="17" spans="1:16" ht="62" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="20">
+        <v>48000</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="25">
+        <v>138708</v>
+      </c>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="19">
+        <v>10</v>
+      </c>
+      <c r="M18" s="19">
+        <v>2025</v>
+      </c>
+      <c r="N18" s="21">
+        <v>0</v>
+      </c>
+      <c r="O18" s="22"/>
+      <c r="P18" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="18">
+        <v>2</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="20">
+        <f>48660+2000000+35000</f>
+        <v>2083660</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="25">
+        <v>0</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="19">
+        <v>15</v>
+      </c>
+      <c r="M19" s="19">
+        <v>2025</v>
+      </c>
+      <c r="N19" s="21"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="18">
+        <v>3</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="20">
+        <f>50000*4+12*25000</f>
+        <v>500000</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="25">
+        <v>2059819</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="19">
+        <v>15</v>
+      </c>
+      <c r="M20" s="19">
+        <v>2026</v>
+      </c>
+      <c r="N20" s="21">
+        <v>-15000</v>
+      </c>
+      <c r="O20" s="22"/>
+      <c r="P20" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18">
+        <v>4</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="20">
+        <v>275000</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="25">
+        <v>230692</v>
+      </c>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="19">
+        <v>20</v>
+      </c>
+      <c r="M21" s="19">
+        <v>2025</v>
+      </c>
+      <c r="N21" s="21"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="18">
+        <v>5</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="20">
+        <f>1200000/1000*2400</f>
+        <v>2880000</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="25">
+        <v>572081</v>
+      </c>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="19">
+        <v>20</v>
+      </c>
+      <c r="M22" s="19">
+        <v>2028</v>
+      </c>
+      <c r="N22" s="21"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="18">
+        <v>6</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="20">
+        <v>1300000</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="25">
+        <v>108695</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="19">
+        <v>15</v>
+      </c>
+      <c r="M23" s="19">
+        <v>2025</v>
+      </c>
+      <c r="N23" s="21"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="18">
+        <v>7</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="20">
+        <v>120000</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="25">
+        <v>19881</v>
+      </c>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="19">
+        <v>20</v>
+      </c>
+      <c r="M24" s="19">
+        <v>2025</v>
+      </c>
+      <c r="N24" s="21"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="18">
+        <v>8</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="20">
+        <f>39790*200</f>
+        <v>7958000</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="25">
+        <v>215217</v>
+      </c>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="19">
+        <v>35</v>
+      </c>
+      <c r="M25" s="19">
+        <v>2029</v>
+      </c>
+      <c r="N25" s="21"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="18">
+        <v>9</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="20">
+        <v>400000</v>
+      </c>
+      <c r="H26" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="25">
+        <v>169502</v>
+      </c>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="19">
+        <v>25</v>
+      </c>
+      <c r="M26" s="19">
+        <v>2030</v>
+      </c>
+      <c r="N26" s="21"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="18">
+        <v>9.1</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="20">
+        <f>3500*2*28</f>
+        <v>196000</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="25">
+        <v>16093</v>
+      </c>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="19">
+        <v>15</v>
+      </c>
+      <c r="M27" s="19">
+        <v>2025</v>
+      </c>
+      <c r="N27" s="21"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="18">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="20">
+        <f>6*350000</f>
+        <v>2100000</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="25">
+        <v>32529</v>
+      </c>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="19">
+        <v>35</v>
+      </c>
+      <c r="M28" s="19">
+        <v>2025</v>
+      </c>
+      <c r="N28" s="21"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="18">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="20">
+        <v>54100000</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" s="25">
+        <v>525655</v>
+      </c>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="19">
+        <v>40</v>
+      </c>
+      <c r="M29" s="19">
+        <v>2035</v>
+      </c>
+      <c r="N29" s="21"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="18">
+        <v>9.4</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="20">
+        <f>1300*1500</f>
+        <v>1950000</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="25">
+        <v>383791</v>
+      </c>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="19">
+        <v>35</v>
+      </c>
+      <c r="M30" s="19">
+        <v>2030</v>
+      </c>
+      <c r="N30" s="21"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="31" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D31" s="19"/>
@@ -1863,38 +2913,33 @@
       <c r="P43" s="16"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:P30">
-    <sortCondition ref="C18:C30"/>
-  </sortState>
   <mergeCells count="1">
     <mergeCell ref="D4:I15"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O28:O33 F31:F44 H31:H43" xr:uid="{19480D23-33C3-4743-91EA-3363E4F8A8EB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26 H26 F28 O18:O30" xr:uid="{0366DE21-3496-4E40-9387-7703B03A7285}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O34:O43 O18:O27 F26 F28:F29" xr:uid="{25478E18-0184-44CC-B842-F228497F826A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H43 F31:F44 O31:O43" xr:uid="{194B9743-F40C-45C2-8612-5F9A36B1FC75}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F74E3BBC-93B3-4149-AA4B-B052653A51FA}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5AC8DA89-CE43-4B7E-8116-98C9A6F06203}">
+          <x14:formula1>
+            <xm:f>Sheet1!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B31:B43</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{848347CF-9068-42E1-8071-4F7B3BAE5274}">
           <x14:formula1>
             <xm:f>Sheet1!$A$1:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B44</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D12C665F-453A-4F1E-8EAE-C130CC2C9B89}">
-          <x14:formula1>
-            <xm:f>Sheet1!$A$1:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>B31:B43</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1902,45 +2947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2E54ED-FA3E-404F-B8C1-A4273C92F2A2}">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7677677-E1F4-40FF-B8C0-372192DBA3AE}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -2339,7 +3346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7EF8B7-F220-45B5-AB65-F2AF33268208}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -2348,6 +3355,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="5" width="20.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>